<commit_message>
added legend to input tables
</commit_message>
<xml_diff>
--- a/correlations/spreadsheets/results.xlsx
+++ b/correlations/spreadsheets/results.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1590" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1632" uniqueCount="36">
   <si>
     <t>starting input</t>
   </si>
@@ -83,6 +83,48 @@
   </si>
   <si>
     <t>1111</t>
+  </si>
+  <si>
+    <t>Field</t>
+  </si>
+  <si>
+    <t>Explanation</t>
+  </si>
+  <si>
+    <t>Old values</t>
+  </si>
+  <si>
+    <t>New values</t>
+  </si>
+  <si>
+    <t>AB change ID</t>
+  </si>
+  <si>
+    <t>Input change ID</t>
+  </si>
+  <si>
+    <t>Hamming distance</t>
+  </si>
+  <si>
+    <t>toggles</t>
+  </si>
+  <si>
+    <t>old values of the inputs before the new inputs are passed (a b r0 r1). E.g. 0110 represents a=0, b=1, r0=1, r1=0</t>
+  </si>
+  <si>
+    <t>old values of the inputs (a b r0 r1). E.g. 0110 represents a=0, b=1, r0=1, r1=0</t>
+  </si>
+  <si>
+    <t>Unique ID for each different change of the old values of a and b</t>
+  </si>
+  <si>
+    <t>Unique ID for each different change of the old values of all inputs</t>
+  </si>
+  <si>
+    <t>Hamming distance between old and new values of the inputs</t>
+  </si>
+  <si>
+    <t>Number of toggles the output performs transitioning from the old to the new values</t>
   </si>
 </sst>
 </file>
@@ -440,13 +482,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F257"/>
+  <dimension ref="A1:J257"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -465,8 +507,14 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="I1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -485,8 +533,14 @@
       <c r="F2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="I2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -505,8 +559,14 @@
       <c r="F3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="I3" t="s">
+        <v>25</v>
+      </c>
+      <c r="J3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -525,8 +585,14 @@
       <c r="F4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="I4" t="s">
+        <v>26</v>
+      </c>
+      <c r="J4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -545,8 +611,14 @@
       <c r="F5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="I5" t="s">
+        <v>27</v>
+      </c>
+      <c r="J5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -565,8 +637,14 @@
       <c r="F6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="I6" t="s">
+        <v>28</v>
+      </c>
+      <c r="J6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -585,8 +663,14 @@
       <c r="F7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="I7" t="s">
+        <v>29</v>
+      </c>
+      <c r="J7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -606,7 +690,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:10">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -626,7 +710,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:10">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -646,7 +730,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:10">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -666,7 +750,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:10">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -686,7 +770,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:10">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -706,7 +790,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:10">
       <c r="A14" t="s">
         <v>6</v>
       </c>
@@ -726,7 +810,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:10">
       <c r="A15" t="s">
         <v>6</v>
       </c>
@@ -746,7 +830,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:10">
       <c r="A16" t="s">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
inserted charts in excel spreadsheet
</commit_message>
<xml_diff>
--- a/correlations/spreadsheets/results.xlsx
+++ b/correlations/spreadsheets/results.xlsx
@@ -7,16 +7,62 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Correlation matrix" sheetId="1" r:id="rId1"/>
+    <sheet name="Toggles no del" sheetId="2" r:id="rId2"/>
+    <sheet name="Toggles del" sheetId="3" r:id="rId3"/>
+    <sheet name="Toggles input del" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+  <si>
+    <t>HW a</t>
+  </si>
+  <si>
+    <t>HW b</t>
+  </si>
+  <si>
+    <t>HW ab</t>
+  </si>
+  <si>
+    <t>HD a</t>
+  </si>
+  <si>
+    <t>HD b</t>
+  </si>
+  <si>
+    <t>HD ab</t>
+  </si>
+  <si>
+    <t>no delays</t>
+  </si>
+  <si>
+    <t>gate delays</t>
+  </si>
+  <si>
+    <t>gate+inputs delay</t>
+  </si>
+  <si>
+    <t>Toggles</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -32,7 +78,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -40,12 +86,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -53,6 +117,336 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'Toggles no del'!$B$2:$B$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>128</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="50010001"/>
+        <c:axId val="50010002"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="50010001"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50010002"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="50010002"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50010001"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'Toggles del'!$B$2:$B$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>48</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="50020001"/>
+        <c:axId val="50020002"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="50020001"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50020002"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="50020002"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50020001"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'Toggles input del'!$B$2:$B$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>112</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="50030001"/>
+        <c:axId val="50030002"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="50030001"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50030002"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="50030002"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50030001"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -340,12 +734,231 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3">
+        <v>0.1796053020267749</v>
+      </c>
+      <c r="C3">
+        <v>0.1796053020267749</v>
+      </c>
+      <c r="D3">
+        <v>0.3110855084191276</v>
+      </c>
+      <c r="E3">
+        <v>0.1796053020267749</v>
+      </c>
+      <c r="F3">
+        <v>0.1796053020267749</v>
+      </c>
+      <c r="G3">
+        <v>0.6956083436402525</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0.3015113445777636</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0.2335496832484569</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>128</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
experiment with only one delayed input. Added observations to README
</commit_message>
<xml_diff>
--- a/correlations/spreadsheets/results.xlsx
+++ b/correlations/spreadsheets/results.xlsx
@@ -280,21 +280,18 @@
           <c:order val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>'Toggles input del'!$B$2:$B$5</c:f>
+              <c:f>'Toggles input del'!$B$2:$B$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>48</c:v>
+                  <c:v>96</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>112</c:v>
+                  <c:v>128</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>16</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -820,13 +817,13 @@
         <v>0</v>
       </c>
       <c r="E4">
-        <v>0.3015113445777636</v>
+        <v>0.3779644730092272</v>
       </c>
       <c r="F4">
         <v>0</v>
       </c>
       <c r="G4">
-        <v>0.2335496832484569</v>
+        <v>0.29277002188456</v>
       </c>
     </row>
   </sheetData>
@@ -914,7 +911,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -930,7 +927,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>48</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -938,7 +935,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>112</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -946,15 +943,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="1">
-        <v>3</v>
-      </c>
-      <c r="B5">
-        <v>16</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
experiment with only one delayed input cntd.
</commit_message>
<xml_diff>
--- a/correlations/spreadsheets/results.xlsx
+++ b/correlations/spreadsheets/results.xlsx
@@ -280,18 +280,21 @@
           <c:order val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>'Toggles input del'!$B$2:$B$4</c:f>
+              <c:f>'Toggles input del'!$B$2:$B$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>96</c:v>
+                  <c:v>72</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>128</c:v>
+                  <c:v>120</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>32</c:v>
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -808,22 +811,22 @@
         <v>8</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>0.3162277660168379</v>
       </c>
       <c r="C4">
         <v>0</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>0.1825741858350554</v>
       </c>
       <c r="E4">
-        <v>0.3779644730092272</v>
+        <v>0.3162277660168379</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>0.3162277660168379</v>
       </c>
       <c r="G4">
-        <v>0.29277002188456</v>
+        <v>0.4898979485566357</v>
       </c>
     </row>
   </sheetData>
@@ -911,7 +914,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -927,7 +930,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>96</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -935,7 +938,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>128</v>
+        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -943,7 +946,15 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>32</v>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new osservations for case with input delay. Summary in README.md
</commit_message>
<xml_diff>
--- a/correlations/spreadsheets/results.xlsx
+++ b/correlations/spreadsheets/results.xlsx
@@ -280,21 +280,18 @@
           <c:order val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>'Toggles input del'!$B$2:$B$5</c:f>
+              <c:f>'Toggles input del'!$B$2:$B$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>72</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>120</c:v>
+                  <c:v>128</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>56</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -811,22 +808,22 @@
         <v>8</v>
       </c>
       <c r="B4">
-        <v>0.3162277660168379</v>
+        <v>0.1796053020267749</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>0.1796053020267749</v>
       </c>
       <c r="D4">
-        <v>0.1825741858350554</v>
+        <v>0.3110855084191276</v>
       </c>
       <c r="E4">
-        <v>0.3162277660168379</v>
+        <v>0.1796053020267749</v>
       </c>
       <c r="F4">
-        <v>0.3162277660168379</v>
+        <v>0.1796053020267749</v>
       </c>
       <c r="G4">
-        <v>0.4898979485566357</v>
+        <v>0.6956083436402525</v>
       </c>
     </row>
   </sheetData>
@@ -914,7 +911,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -930,7 +927,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>72</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -938,7 +935,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>120</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -946,15 +943,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="1">
-        <v>3</v>
-      </c>
-      <c r="B5">
-        <v>8</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
scripts separated from main. added configuration file for delays
</commit_message>
<xml_diff>
--- a/correlations/spreadsheets/results.xlsx
+++ b/correlations/spreadsheets/results.xlsx
@@ -205,18 +205,21 @@
           <c:order val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>'Toggles del'!$B$2:$B$4</c:f>
+              <c:f>'Toggles del'!$B$2:$B$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>80</c:v>
+                  <c:v>72</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>128</c:v>
+                  <c:v>120</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>48</c:v>
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -280,18 +283,21 @@
           <c:order val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>'Toggles input del'!$B$2:$B$4</c:f>
+              <c:f>'Toggles input del'!$B$2:$B$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>80</c:v>
+                  <c:v>72</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>128</c:v>
+                  <c:v>120</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>48</c:v>
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -785,22 +791,22 @@
         <v>7</v>
       </c>
       <c r="B3">
-        <v>0.1796053020267749</v>
+        <v>0.3162277660168379</v>
       </c>
       <c r="C3">
-        <v>0.1796053020267749</v>
+        <v>0</v>
       </c>
       <c r="D3">
-        <v>0.3110855084191276</v>
+        <v>0.1825741858350554</v>
       </c>
       <c r="E3">
-        <v>0.1796053020267749</v>
+        <v>0.3162277660168379</v>
       </c>
       <c r="F3">
-        <v>0.1796053020267749</v>
+        <v>0.3162277660168379</v>
       </c>
       <c r="G3">
-        <v>0.6956083436402525</v>
+        <v>0.4898979485566357</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -808,22 +814,22 @@
         <v>8</v>
       </c>
       <c r="B4">
-        <v>0.1796053020267749</v>
+        <v>0.3162277660168379</v>
       </c>
       <c r="C4">
-        <v>0.1796053020267749</v>
+        <v>0</v>
       </c>
       <c r="D4">
-        <v>0.3110855084191276</v>
+        <v>0.1825741858350554</v>
       </c>
       <c r="E4">
-        <v>0.1796053020267749</v>
+        <v>0.3162277660168379</v>
       </c>
       <c r="F4">
-        <v>0.1796053020267749</v>
+        <v>0.3162277660168379</v>
       </c>
       <c r="G4">
-        <v>0.6956083436402525</v>
+        <v>0.4898979485566357</v>
       </c>
     </row>
   </sheetData>
@@ -868,7 +874,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -884,7 +890,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>80</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -892,7 +898,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>128</v>
+        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -900,7 +906,15 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>48</v>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -911,7 +925,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -927,7 +941,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>80</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -935,7 +949,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>128</v>
+        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -943,7 +957,15 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>48</v>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added interface for any type of gadget. Correlation calculation not working. TB needs to be modified
</commit_message>
<xml_diff>
--- a/correlations/spreadsheets/results.xlsx
+++ b/correlations/spreadsheets/results.xlsx
@@ -205,21 +205,15 @@
           <c:order val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>'Toggles del'!$B$2:$B$5</c:f>
+              <c:f>'Toggles del'!$B$2:$B$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>72</c:v>
+                  <c:v>128</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>120</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>56</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8</c:v>
+                  <c:v>128</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -283,21 +277,15 @@
           <c:order val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>'Toggles input del'!$B$2:$B$5</c:f>
+              <c:f>'Toggles input del'!$B$2:$B$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>72</c:v>
+                  <c:v>128</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>120</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>56</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8</c:v>
+                  <c:v>128</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -783,7 +771,7 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>0.06454972243679027</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -791,22 +779,22 @@
         <v>7</v>
       </c>
       <c r="B3">
-        <v>0.3162277660168379</v>
+        <v>0</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3">
-        <v>0.1825741858350554</v>
+        <v>0</v>
       </c>
       <c r="E3">
-        <v>0.3162277660168379</v>
+        <v>0</v>
       </c>
       <c r="F3">
-        <v>0.3162277660168379</v>
+        <v>0</v>
       </c>
       <c r="G3">
-        <v>0.4898979485566357</v>
+        <v>0.06454972243679027</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -814,22 +802,22 @@
         <v>8</v>
       </c>
       <c r="B4">
-        <v>0.3162277660168379</v>
+        <v>0</v>
       </c>
       <c r="C4">
         <v>0</v>
       </c>
       <c r="D4">
-        <v>0.1825741858350554</v>
+        <v>0</v>
       </c>
       <c r="E4">
-        <v>0.3162277660168379</v>
+        <v>0</v>
       </c>
       <c r="F4">
-        <v>0.3162277660168379</v>
+        <v>0</v>
       </c>
       <c r="G4">
-        <v>0.4898979485566357</v>
+        <v>0.06454972243679027</v>
       </c>
     </row>
   </sheetData>
@@ -874,7 +862,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -890,7 +878,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>72</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -898,23 +886,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="1">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="1">
-        <v>3</v>
-      </c>
-      <c r="B5">
-        <v>8</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -925,7 +897,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -941,7 +913,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>72</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -949,23 +921,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="1">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="1">
-        <v>3</v>
-      </c>
-      <c r="B5">
-        <v>8</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modified to work with any number of inputs. added possibility to do less simulations but only with PRNG.
</commit_message>
<xml_diff>
--- a/correlations/spreadsheets/results.xlsx
+++ b/correlations/spreadsheets/results.xlsx
@@ -17,24 +17,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
-    <t>HW a</t>
+    <t>HW input0</t>
   </si>
   <si>
-    <t>HW b</t>
+    <t>HW input1</t>
   </si>
   <si>
-    <t>HW ab</t>
+    <t>HD input0</t>
   </si>
   <si>
-    <t>HD a</t>
-  </si>
-  <si>
-    <t>HD b</t>
-  </si>
-  <si>
-    <t>HD ab</t>
+    <t>HD input1</t>
   </si>
   <si>
     <t>no delays</t>
@@ -138,10 +132,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>128</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>128</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -205,15 +199,18 @@
           <c:order val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>'Toggles del'!$B$2:$B$3</c:f>
+              <c:f>'Toggles del'!$B$2:$B$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>128</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>128</c:v>
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>24</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -277,15 +274,18 @@
           <c:order val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>'Toggles input del'!$B$2:$B$3</c:f>
+              <c:f>'Toggles input del'!$B$2:$B$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>128</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>128</c:v>
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>24</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -725,13 +725,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:5">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -744,80 +744,56 @@
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="B2">
+        <v>-0.1326070442732927</v>
+      </c>
+      <c r="C2">
+        <v>0.0440713778829488</v>
+      </c>
+      <c r="D2">
+        <v>0.0008442028516211154</v>
+      </c>
+      <c r="E2">
+        <v>0.05107738391369917</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="1" t="s">
+      <c r="B3">
+        <v>0.2068697284125937</v>
+      </c>
+      <c r="C3">
+        <v>-0.1087668027104684</v>
+      </c>
+      <c r="D3">
+        <v>0.07630319080522027</v>
+      </c>
+      <c r="E3">
+        <v>-0.1175844557494744</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>0.06454972243679027</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>0.06454972243679027</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="B4">
-        <v>0</v>
+        <v>0.2068697284125937</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>-0.1087668027104684</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>0.07630319080522027</v>
       </c>
       <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>0.06454972243679027</v>
+        <v>-0.1175844557494744</v>
       </c>
     </row>
   </sheetData>
@@ -835,7 +811,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="B1" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -843,7 +819,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>128</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -851,7 +827,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>128</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -862,7 +838,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -870,7 +846,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="B1" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -878,7 +854,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>128</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -886,7 +862,15 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>128</v>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -897,7 +881,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -905,7 +889,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="B1" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -913,7 +897,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>128</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -921,7 +905,15 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>128</v>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
works with gadget with any number of inputs, with full simulation or partial. also added register level in the gadget interface
</commit_message>
<xml_diff>
--- a/correlations/spreadsheets/results.xlsx
+++ b/correlations/spreadsheets/results.xlsx
@@ -132,10 +132,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>68</c:v>
+                  <c:v>128</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>53</c:v>
+                  <c:v>128</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -204,13 +204,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>68</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>29</c:v>
+                  <c:v>128</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>24</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -279,13 +279,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>68</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>29</c:v>
+                  <c:v>128</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>24</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -750,16 +750,16 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>-0.1326070442732927</v>
+        <v>0</v>
       </c>
       <c r="C2">
-        <v>0.0440713778829488</v>
+        <v>0</v>
       </c>
       <c r="D2">
-        <v>0.0008442028516211154</v>
+        <v>0</v>
       </c>
       <c r="E2">
-        <v>0.05107738391369917</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -767,16 +767,16 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>0.2068697284125937</v>
+        <v>0.1796053020267749</v>
       </c>
       <c r="C3">
-        <v>-0.1087668027104684</v>
+        <v>0.1796053020267749</v>
       </c>
       <c r="D3">
-        <v>0.07630319080522027</v>
+        <v>0.1796053020267749</v>
       </c>
       <c r="E3">
-        <v>-0.1175844557494744</v>
+        <v>0.1796053020267749</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -784,16 +784,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>0.2068697284125937</v>
+        <v>0.1796053020267749</v>
       </c>
       <c r="C4">
-        <v>-0.1087668027104684</v>
+        <v>0.1796053020267749</v>
       </c>
       <c r="D4">
-        <v>0.07630319080522027</v>
+        <v>0.1796053020267749</v>
       </c>
       <c r="E4">
-        <v>-0.1175844557494744</v>
+        <v>0.1796053020267749</v>
       </c>
     </row>
   </sheetData>
@@ -819,7 +819,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>68</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -827,7 +827,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>53</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -854,7 +854,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>68</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -862,7 +862,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>29</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -870,7 +870,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>24</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -897,7 +897,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>68</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -905,7 +905,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>29</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -913,7 +913,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>24</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
separated selection function and consume models into two separate functions for easier modification
</commit_message>
<xml_diff>
--- a/correlations/spreadsheets/results.xlsx
+++ b/correlations/spreadsheets/results.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>HW input0</t>
   </si>
@@ -25,10 +25,46 @@
     <t>HW input1</t>
   </si>
   <si>
+    <t>HW input2</t>
+  </si>
+  <si>
+    <t>HW input3</t>
+  </si>
+  <si>
+    <t>HW input4</t>
+  </si>
+  <si>
+    <t>HW input5</t>
+  </si>
+  <si>
+    <t>HW input6</t>
+  </si>
+  <si>
+    <t>HW input7</t>
+  </si>
+  <si>
     <t>HD input0</t>
   </si>
   <si>
     <t>HD input1</t>
+  </si>
+  <si>
+    <t>HD input2</t>
+  </si>
+  <si>
+    <t>HD input3</t>
+  </si>
+  <si>
+    <t>HD input4</t>
+  </si>
+  <si>
+    <t>HD input5</t>
+  </si>
+  <si>
+    <t>HD input6</t>
+  </si>
+  <si>
+    <t>HD input7</t>
   </si>
   <si>
     <t>no delays</t>
@@ -127,15 +163,18 @@
           <c:order val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>'Toggles no del'!$B$2:$B$3</c:f>
+              <c:f>'Toggles no del'!$B$2:$B$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>128</c:v>
+                  <c:v>67</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>128</c:v>
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -199,18 +238,21 @@
           <c:order val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>'Toggles del'!$B$2:$B$4</c:f>
+              <c:f>'Toggles del'!$B$2:$B$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>80</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>128</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>48</c:v>
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -274,18 +316,21 @@
           <c:order val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>'Toggles input del'!$B$2:$B$4</c:f>
+              <c:f>'Toggles input del'!$B$2:$B$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>80</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>128</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>48</c:v>
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -725,13 +770,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:Q4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:17">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -744,56 +789,200 @@
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="B2">
+        <v>0.1036951694730425</v>
+      </c>
+      <c r="C2">
+        <v>-0.3246172270321178</v>
+      </c>
+      <c r="D2">
+        <v>-0.5388159060803247</v>
+      </c>
+      <c r="E2">
+        <v>0.3110855084191276</v>
+      </c>
+      <c r="F2">
+        <v>0.1796053020267749</v>
+      </c>
+      <c r="G2">
+        <v>-0.5388159060803247</v>
+      </c>
+      <c r="H2">
+        <v>-0.5388159060803247</v>
+      </c>
+      <c r="I2">
+        <v>0.5184758473652127</v>
+      </c>
+      <c r="J2">
+        <v>-0.6956083436402525</v>
+      </c>
+      <c r="K2">
+        <v>0.5184758473652127</v>
+      </c>
+      <c r="L2">
+        <v>0.1796053020267749</v>
+      </c>
+      <c r="M2">
+        <v>0.5388159060803247</v>
+      </c>
+      <c r="N2">
+        <v>-0.5388159060803247</v>
+      </c>
+      <c r="O2">
+        <v>0.1036951694730425</v>
+      </c>
+      <c r="P2">
+        <v>-0.7258661863112977</v>
+      </c>
+      <c r="Q2">
+        <v>0.5388159060803247</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
+      <c r="A3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3">
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="C3">
+        <v>-0.149071198499986</v>
+      </c>
+      <c r="D3">
+        <v>-0.5773502691896257</v>
+      </c>
+      <c r="E3">
+        <v>-0.1111111111111111</v>
+      </c>
+      <c r="F3">
         <v>0</v>
       </c>
-      <c r="C2">
+      <c r="G3">
+        <v>-0.3849001794597505</v>
+      </c>
+      <c r="H3">
+        <v>-0.3849001794597505</v>
+      </c>
+      <c r="I3">
+        <v>0.5555555555555556</v>
+      </c>
+      <c r="J3">
+        <v>-0.7453559924999299</v>
+      </c>
+      <c r="K3">
+        <v>0.5555555555555556</v>
+      </c>
+      <c r="L3">
+        <v>-0.1924500897298753</v>
+      </c>
+      <c r="M3">
+        <v>0.3849001794597505</v>
+      </c>
+      <c r="N3">
+        <v>-0.5773502691896257</v>
+      </c>
+      <c r="O3">
+        <v>-0.1111111111111111</v>
+      </c>
+      <c r="P3">
+        <v>-0.5555555555555556</v>
+      </c>
+      <c r="Q3">
+        <v>0.5773502691896257</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17">
+      <c r="A4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4">
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="C4">
+        <v>-0.149071198499986</v>
+      </c>
+      <c r="D4">
+        <v>-0.5773502691896257</v>
+      </c>
+      <c r="E4">
+        <v>-0.1111111111111111</v>
+      </c>
+      <c r="F4">
         <v>0</v>
       </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3">
-        <v>0.1796053020267749</v>
-      </c>
-      <c r="C3">
-        <v>0.1796053020267749</v>
-      </c>
-      <c r="D3">
-        <v>0.1796053020267749</v>
-      </c>
-      <c r="E3">
-        <v>0.1796053020267749</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4">
-        <v>0.1796053020267749</v>
-      </c>
-      <c r="C4">
-        <v>0.1796053020267749</v>
-      </c>
-      <c r="D4">
-        <v>0.1796053020267749</v>
-      </c>
-      <c r="E4">
-        <v>0.1796053020267749</v>
+      <c r="G4">
+        <v>-0.3849001794597505</v>
+      </c>
+      <c r="H4">
+        <v>-0.3849001794597505</v>
+      </c>
+      <c r="I4">
+        <v>0.5555555555555556</v>
+      </c>
+      <c r="J4">
+        <v>-0.7453559924999299</v>
+      </c>
+      <c r="K4">
+        <v>0.5555555555555556</v>
+      </c>
+      <c r="L4">
+        <v>-0.1924500897298753</v>
+      </c>
+      <c r="M4">
+        <v>0.3849001794597505</v>
+      </c>
+      <c r="N4">
+        <v>-0.5773502691896257</v>
+      </c>
+      <c r="O4">
+        <v>-0.1111111111111111</v>
+      </c>
+      <c r="P4">
+        <v>-0.5555555555555556</v>
+      </c>
+      <c r="Q4">
+        <v>0.5773502691896257</v>
       </c>
     </row>
   </sheetData>
@@ -802,41 +991,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="B1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>128</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -846,7 +1000,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -854,7 +1008,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>80</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -862,7 +1016,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>128</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -870,7 +1024,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>48</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -879,9 +1033,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -889,7 +1043,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -897,7 +1051,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>80</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -905,7 +1059,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>128</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -913,7 +1067,66 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>48</v>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="B1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
random input generation moved to python script. Testbench reads the generated inputs => better random generation
</commit_message>
<xml_diff>
--- a/correlations/spreadsheets/results.xlsx
+++ b/correlations/spreadsheets/results.xlsx
@@ -168,13 +168,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>67</c:v>
+                  <c:v>310</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>51</c:v>
+                  <c:v>248</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -243,16 +243,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>7</c:v>
+                  <c:v>263</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>42</c:v>
+                  <c:v>218</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>58</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>14</c:v>
+                  <c:v>59</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -321,16 +321,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>7</c:v>
+                  <c:v>263</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>42</c:v>
+                  <c:v>218</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>58</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>14</c:v>
+                  <c:v>59</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -831,52 +831,52 @@
         <v>16</v>
       </c>
       <c r="B2">
-        <v>0.1036951694730425</v>
+        <v>-0.0578566758318202</v>
       </c>
       <c r="C2">
-        <v>-0.3246172270321178</v>
+        <v>0.01572563675836635</v>
       </c>
       <c r="D2">
-        <v>-0.5388159060803247</v>
+        <v>0.02217052873220555</v>
       </c>
       <c r="E2">
-        <v>0.3110855084191276</v>
+        <v>-0.03112808543034129</v>
       </c>
       <c r="F2">
-        <v>0.1796053020267749</v>
+        <v>0.009506676583047996</v>
       </c>
       <c r="G2">
-        <v>-0.5388159060803247</v>
+        <v>-0.04376408419878811</v>
       </c>
       <c r="H2">
-        <v>-0.5388159060803247</v>
+        <v>-0.0133642952007395</v>
       </c>
       <c r="I2">
-        <v>0.5184758473652127</v>
+        <v>0.06926441168555347</v>
       </c>
       <c r="J2">
-        <v>-0.6956083436402525</v>
+        <v>0.06041161340274066</v>
       </c>
       <c r="K2">
-        <v>0.5184758473652127</v>
+        <v>0.02852866041351129</v>
       </c>
       <c r="L2">
-        <v>0.1796053020267749</v>
+        <v>-0.06671255020778472</v>
       </c>
       <c r="M2">
-        <v>0.5388159060803247</v>
+        <v>-0.07939371386395846</v>
       </c>
       <c r="N2">
-        <v>-0.5388159060803247</v>
+        <v>-0.0136233376951211</v>
       </c>
       <c r="O2">
-        <v>0.1036951694730425</v>
+        <v>-0.02091772575958519</v>
       </c>
       <c r="P2">
-        <v>-0.7258661863112977</v>
+        <v>-0.07196674847465961</v>
       </c>
       <c r="Q2">
-        <v>0.5388159060803247</v>
+        <v>-0.09351063661446735</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -884,52 +884,52 @@
         <v>17</v>
       </c>
       <c r="B3">
-        <v>0.1111111111111111</v>
+        <v>-0.02796824689522253</v>
       </c>
       <c r="C3">
-        <v>-0.149071198499986</v>
+        <v>0.04783872147277625</v>
       </c>
       <c r="D3">
-        <v>-0.5773502691896257</v>
+        <v>0.03070688879037094</v>
       </c>
       <c r="E3">
-        <v>-0.1111111111111111</v>
+        <v>-0.01978241853564501</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>0.0375192878561945</v>
       </c>
       <c r="G3">
-        <v>-0.3849001794597505</v>
+        <v>-0.05734591371064292</v>
       </c>
       <c r="H3">
-        <v>-0.3849001794597505</v>
+        <v>0.009550133086173319</v>
       </c>
       <c r="I3">
-        <v>0.5555555555555556</v>
+        <v>0.006139371269682767</v>
       </c>
       <c r="J3">
-        <v>-0.7453559924999299</v>
+        <v>0.03069759915506819</v>
       </c>
       <c r="K3">
-        <v>0.5555555555555556</v>
+        <v>0.006823753064526763</v>
       </c>
       <c r="L3">
-        <v>-0.1924500897298753</v>
+        <v>-0.0341084435056314</v>
       </c>
       <c r="M3">
-        <v>0.3849001794597505</v>
+        <v>-0.0341187653226344</v>
       </c>
       <c r="N3">
-        <v>-0.5773502691896257</v>
+        <v>-0.004104351229156675</v>
       </c>
       <c r="O3">
-        <v>-0.1111111111111111</v>
+        <v>0.004775875553192661</v>
       </c>
       <c r="P3">
-        <v>-0.5555555555555556</v>
+        <v>-0.06006138954307796</v>
       </c>
       <c r="Q3">
-        <v>0.5773502691896257</v>
+        <v>-0.03888927236171197</v>
       </c>
     </row>
     <row r="4" spans="1:17">
@@ -937,52 +937,52 @@
         <v>18</v>
       </c>
       <c r="B4">
-        <v>0.1111111111111111</v>
+        <v>-0.02796824689522253</v>
       </c>
       <c r="C4">
-        <v>-0.149071198499986</v>
+        <v>0.04783872147277625</v>
       </c>
       <c r="D4">
-        <v>-0.5773502691896257</v>
+        <v>0.03070688879037094</v>
       </c>
       <c r="E4">
-        <v>-0.1111111111111111</v>
+        <v>-0.01978241853564501</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>0.0375192878561945</v>
       </c>
       <c r="G4">
-        <v>-0.3849001794597505</v>
+        <v>-0.05734591371064292</v>
       </c>
       <c r="H4">
-        <v>-0.3849001794597505</v>
+        <v>0.009550133086173319</v>
       </c>
       <c r="I4">
-        <v>0.5555555555555556</v>
+        <v>0.006139371269682767</v>
       </c>
       <c r="J4">
-        <v>-0.7453559924999299</v>
+        <v>0.03069759915506819</v>
       </c>
       <c r="K4">
-        <v>0.5555555555555556</v>
+        <v>0.006823753064526763</v>
       </c>
       <c r="L4">
-        <v>-0.1924500897298753</v>
+        <v>-0.0341084435056314</v>
       </c>
       <c r="M4">
-        <v>0.3849001794597505</v>
+        <v>-0.0341187653226344</v>
       </c>
       <c r="N4">
-        <v>-0.5773502691896257</v>
+        <v>-0.004104351229156675</v>
       </c>
       <c r="O4">
-        <v>-0.1111111111111111</v>
+        <v>0.004775875553192661</v>
       </c>
       <c r="P4">
-        <v>-0.5555555555555556</v>
+        <v>-0.06006138954307796</v>
       </c>
       <c r="Q4">
-        <v>0.5773502691896257</v>
+        <v>-0.03888927236171197</v>
       </c>
     </row>
   </sheetData>
@@ -1008,7 +1008,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>67</v>
+        <v>310</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1016,7 +1016,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>51</v>
+        <v>248</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1024,7 +1024,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -1051,7 +1051,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>7</v>
+        <v>263</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1059,7 +1059,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>42</v>
+        <v>218</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1067,7 +1067,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>58</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1075,7 +1075,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>14</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1102,7 +1102,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>7</v>
+        <v>263</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1110,7 +1110,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>42</v>
+        <v>218</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1118,7 +1118,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>58</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1126,7 +1126,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>14</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
config file is now passed as parameter in order to be able to have one config file for every gadget in src
</commit_message>
<xml_diff>
--- a/correlations/spreadsheets/results.xlsx
+++ b/correlations/spreadsheets/results.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
     <t>HW input0</t>
   </si>
@@ -25,46 +25,10 @@
     <t>HW input1</t>
   </si>
   <si>
-    <t>HW input2</t>
-  </si>
-  <si>
-    <t>HW input3</t>
-  </si>
-  <si>
-    <t>HW input4</t>
-  </si>
-  <si>
-    <t>HW input5</t>
-  </si>
-  <si>
-    <t>HW input6</t>
-  </si>
-  <si>
-    <t>HW input7</t>
-  </si>
-  <si>
     <t>HD input0</t>
   </si>
   <si>
     <t>HD input1</t>
-  </si>
-  <si>
-    <t>HD input2</t>
-  </si>
-  <si>
-    <t>HD input3</t>
-  </si>
-  <si>
-    <t>HD input4</t>
-  </si>
-  <si>
-    <t>HD input5</t>
-  </si>
-  <si>
-    <t>HD input6</t>
-  </si>
-  <si>
-    <t>HD input7</t>
   </si>
   <si>
     <t>no delays</t>
@@ -163,18 +127,15 @@
           <c:order val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>'Toggles no del'!$B$2:$B$4</c:f>
+              <c:f>'Toggles no del'!$B$2:$B$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>310</c:v>
+                  <c:v>127</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>248</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>17</c:v>
+                  <c:v>128</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -238,21 +199,18 @@
           <c:order val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>'Toggles del'!$B$2:$B$5</c:f>
+              <c:f>'Toggles del'!$B$2:$B$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>263</c:v>
+                  <c:v>79</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>218</c:v>
+                  <c:v>128</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>35</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>59</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -316,21 +274,18 @@
           <c:order val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>'Toggles input del'!$B$2:$B$5</c:f>
+              <c:f>'Toggles input del'!$B$2:$B$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>263</c:v>
+                  <c:v>79</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>218</c:v>
+                  <c:v>128</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>35</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>59</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -770,13 +725,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:5">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -789,200 +744,56 @@
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="B2">
+        <v>0.003937007874015723</v>
+      </c>
+      <c r="C2">
+        <v>0.003937007874015723</v>
+      </c>
+      <c r="D2">
+        <v>-0.003937007874015723</v>
+      </c>
+      <c r="E2">
+        <v>-0.003937007874015723</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="B3">
+        <v>0.1854742807555382</v>
+      </c>
+      <c r="C3">
+        <v>0.1854742807555382</v>
+      </c>
+      <c r="D3">
+        <v>0.1755634413258522</v>
+      </c>
+      <c r="E3">
+        <v>0.1755634413258529</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17">
-      <c r="A2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2">
-        <v>-0.0578566758318202</v>
-      </c>
-      <c r="C2">
-        <v>0.01572563675836635</v>
-      </c>
-      <c r="D2">
-        <v>0.02217052873220555</v>
-      </c>
-      <c r="E2">
-        <v>-0.03112808543034129</v>
-      </c>
-      <c r="F2">
-        <v>0.009506676583047996</v>
-      </c>
-      <c r="G2">
-        <v>-0.04376408419878811</v>
-      </c>
-      <c r="H2">
-        <v>-0.0133642952007395</v>
-      </c>
-      <c r="I2">
-        <v>0.06926441168555347</v>
-      </c>
-      <c r="J2">
-        <v>0.06041161340274066</v>
-      </c>
-      <c r="K2">
-        <v>0.02852866041351129</v>
-      </c>
-      <c r="L2">
-        <v>-0.06671255020778472</v>
-      </c>
-      <c r="M2">
-        <v>-0.07939371386395846</v>
-      </c>
-      <c r="N2">
-        <v>-0.0136233376951211</v>
-      </c>
-      <c r="O2">
-        <v>-0.02091772575958519</v>
-      </c>
-      <c r="P2">
-        <v>-0.07196674847465961</v>
-      </c>
-      <c r="Q2">
-        <v>-0.09351063661446735</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17">
-      <c r="A3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3">
-        <v>-0.02796824689522253</v>
-      </c>
-      <c r="C3">
-        <v>0.04783872147277625</v>
-      </c>
-      <c r="D3">
-        <v>0.03070688879037094</v>
-      </c>
-      <c r="E3">
-        <v>-0.01978241853564501</v>
-      </c>
-      <c r="F3">
-        <v>0.0375192878561945</v>
-      </c>
-      <c r="G3">
-        <v>-0.05734591371064292</v>
-      </c>
-      <c r="H3">
-        <v>0.009550133086173319</v>
-      </c>
-      <c r="I3">
-        <v>0.006139371269682767</v>
-      </c>
-      <c r="J3">
-        <v>0.03069759915506819</v>
-      </c>
-      <c r="K3">
-        <v>0.006823753064526763</v>
-      </c>
-      <c r="L3">
-        <v>-0.0341084435056314</v>
-      </c>
-      <c r="M3">
-        <v>-0.0341187653226344</v>
-      </c>
-      <c r="N3">
-        <v>-0.004104351229156675</v>
-      </c>
-      <c r="O3">
-        <v>0.004775875553192661</v>
-      </c>
-      <c r="P3">
-        <v>-0.06006138954307796</v>
-      </c>
-      <c r="Q3">
-        <v>-0.03888927236171197</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17">
-      <c r="A4" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="B4">
-        <v>-0.02796824689522253</v>
+        <v>0.1854742807555382</v>
       </c>
       <c r="C4">
-        <v>0.04783872147277625</v>
+        <v>0.1854742807555382</v>
       </c>
       <c r="D4">
-        <v>0.03070688879037094</v>
+        <v>0.1755634413258522</v>
       </c>
       <c r="E4">
-        <v>-0.01978241853564501</v>
-      </c>
-      <c r="F4">
-        <v>0.0375192878561945</v>
-      </c>
-      <c r="G4">
-        <v>-0.05734591371064292</v>
-      </c>
-      <c r="H4">
-        <v>0.009550133086173319</v>
-      </c>
-      <c r="I4">
-        <v>0.006139371269682767</v>
-      </c>
-      <c r="J4">
-        <v>0.03069759915506819</v>
-      </c>
-      <c r="K4">
-        <v>0.006823753064526763</v>
-      </c>
-      <c r="L4">
-        <v>-0.0341084435056314</v>
-      </c>
-      <c r="M4">
-        <v>-0.0341187653226344</v>
-      </c>
-      <c r="N4">
-        <v>-0.004104351229156675</v>
-      </c>
-      <c r="O4">
-        <v>0.004775875553192661</v>
-      </c>
-      <c r="P4">
-        <v>-0.06006138954307796</v>
-      </c>
-      <c r="Q4">
-        <v>-0.03888927236171197</v>
+        <v>0.1755634413258529</v>
       </c>
     </row>
   </sheetData>
@@ -991,6 +802,41 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>128</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -1000,7 +846,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="B1" s="1" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1008,7 +854,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>310</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1016,7 +862,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>248</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1024,7 +870,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>17</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1033,9 +879,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1043,7 +889,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="B1" s="1" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1051,7 +897,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>263</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1059,7 +905,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>218</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1067,66 +913,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="1">
-        <v>3</v>
-      </c>
-      <c r="B5">
-        <v>59</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="B1" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="1">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="1">
-        <v>3</v>
-      </c>
-      <c r="B5">
-        <v>59</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>